<commit_message>
Made small changes to Projektplaungs-stuff
</commit_message>
<xml_diff>
--- a/Projekthandbuch/Planungsdokumente/Gantt_Diagramm.xlsx
+++ b/Projekthandbuch/Planungsdokumente/Gantt_Diagramm.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i589151/repos/webengineering/Projekthandbuch/Planungsdokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{1FE5A28D-4E57-B84D-BE27-6551B69D71FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{8700D260-84FE-6444-ADB5-0AAF5BB02829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3700" yWindow="-17960" windowWidth="15120" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Plan!$A$1:$CF$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>Dauer in Tagen</t>
   </si>
@@ -69,21 +72,6 @@
   </si>
   <si>
     <t>KW 30</t>
-  </si>
-  <si>
-    <t>KW 31</t>
-  </si>
-  <si>
-    <t>KW 32</t>
-  </si>
-  <si>
-    <t>KW 33</t>
-  </si>
-  <si>
-    <t>KW 34</t>
-  </si>
-  <si>
-    <t>KW 35</t>
   </si>
   <si>
     <t>Kick-Off</t>
@@ -835,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DY15"/>
+  <dimension ref="A1:CO15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="61" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="CP9" sqref="CP9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -852,27 +840,27 @@
     <col min="8" max="119" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:129" ht="16">
+    <row r="1" spans="1:93" ht="16">
       <c r="A1" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>1</v>
@@ -973,61 +961,16 @@
       <c r="CD1" s="22"/>
       <c r="CE1" s="22"/>
       <c r="CF1" s="23"/>
-      <c r="CG1" s="21" t="s">
+    </row>
+    <row r="2" spans="1:93" ht="50" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="CH1" s="22"/>
-      <c r="CI1" s="22"/>
-      <c r="CJ1" s="22"/>
-      <c r="CK1" s="22"/>
-      <c r="CL1" s="22"/>
-      <c r="CM1" s="23"/>
-      <c r="CN1" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="CO1" s="22"/>
-      <c r="CP1" s="22"/>
-      <c r="CQ1" s="22"/>
-      <c r="CR1" s="22"/>
-      <c r="CS1" s="22"/>
-      <c r="CT1" s="23"/>
-      <c r="CU1" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="CV1" s="22"/>
-      <c r="CW1" s="22"/>
-      <c r="CX1" s="22"/>
-      <c r="CY1" s="22"/>
-      <c r="CZ1" s="22"/>
-      <c r="DA1" s="23"/>
-      <c r="DB1" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="DC1" s="22"/>
-      <c r="DD1" s="22"/>
-      <c r="DE1" s="22"/>
-      <c r="DF1" s="22"/>
-      <c r="DG1" s="22"/>
-      <c r="DH1" s="23"/>
-      <c r="DI1" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="DJ1" s="22"/>
-      <c r="DK1" s="22"/>
-      <c r="DL1" s="22"/>
-      <c r="DM1" s="22"/>
-      <c r="DN1" s="22"/>
-      <c r="DO1" s="23"/>
-    </row>
-    <row r="2" spans="1:129" ht="50" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2">
         <f>F2-E2</f>
@@ -1040,7 +983,7 @@
         <v>45427</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H2" s="13">
         <v>0</v>
@@ -1207,91 +1150,25 @@
       <c r="CF2" s="14">
         <v>0</v>
       </c>
-      <c r="CG2" s="14">
-        <v>0</v>
-      </c>
-      <c r="CH2" s="14"/>
-      <c r="CI2" s="14"/>
-      <c r="CJ2" s="14"/>
-      <c r="CK2" s="14"/>
-      <c r="CL2" s="14">
-        <v>0</v>
-      </c>
-      <c r="CM2" s="14">
-        <v>0</v>
-      </c>
-      <c r="CN2" s="14">
-        <v>0</v>
-      </c>
-      <c r="CO2" s="14"/>
-      <c r="CP2" s="14"/>
-      <c r="CQ2" s="14"/>
-      <c r="CR2" s="14"/>
-      <c r="CS2" s="14">
-        <v>0</v>
-      </c>
-      <c r="CT2" s="14">
-        <v>0</v>
-      </c>
-      <c r="CU2" s="14">
-        <v>0</v>
-      </c>
-      <c r="CV2" s="14"/>
-      <c r="CW2" s="14"/>
-      <c r="CX2" s="14"/>
-      <c r="CY2" s="14">
-        <v>0</v>
-      </c>
-      <c r="CZ2" s="14"/>
-      <c r="DA2" s="14">
-        <v>0</v>
-      </c>
-      <c r="DB2" s="14">
-        <v>0</v>
-      </c>
-      <c r="DC2" s="14"/>
-      <c r="DD2" s="14"/>
-      <c r="DE2" s="14"/>
-      <c r="DF2" s="14">
-        <v>0</v>
-      </c>
-      <c r="DG2" s="14"/>
-      <c r="DH2" s="14">
-        <v>0</v>
-      </c>
-      <c r="DI2" s="14">
-        <v>0</v>
-      </c>
-      <c r="DJ2" s="14"/>
-      <c r="DK2" s="14"/>
-      <c r="DL2" s="14"/>
-      <c r="DM2" s="14"/>
-      <c r="DN2" s="14">
-        <v>0</v>
-      </c>
-      <c r="DO2" s="14">
-        <v>0</v>
-      </c>
-      <c r="DP2" s="1"/>
-      <c r="DQ2" s="1"/>
-      <c r="DR2" s="1"/>
-      <c r="DS2" s="1"/>
-      <c r="DT2" s="1"/>
-      <c r="DU2" s="1"/>
-      <c r="DV2" s="1"/>
-      <c r="DW2" s="1"/>
-      <c r="DX2" s="1"/>
-      <c r="DY2" s="1"/>
+      <c r="CG2" s="1"/>
+      <c r="CH2" s="1"/>
+      <c r="CI2" s="1"/>
+      <c r="CJ2" s="1"/>
+      <c r="CK2" s="1"/>
+      <c r="CL2" s="1"/>
+      <c r="CM2" s="1"/>
+      <c r="CN2" s="1"/>
+      <c r="CO2" s="1"/>
     </row>
-    <row r="3" spans="1:129" ht="50" customHeight="1">
+    <row r="3" spans="1:93" ht="50" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2">
         <f>F3-E3</f>
@@ -1304,7 +1181,7 @@
         <v>45436</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H3" s="15">
         <v>0</v>
@@ -1495,91 +1372,25 @@
       <c r="CF3" s="14">
         <v>0</v>
       </c>
-      <c r="CG3" s="14">
-        <v>0</v>
-      </c>
-      <c r="CH3" s="14"/>
-      <c r="CI3" s="14"/>
-      <c r="CJ3" s="14"/>
-      <c r="CK3" s="14"/>
-      <c r="CL3" s="14">
-        <v>0</v>
-      </c>
-      <c r="CM3" s="14">
-        <v>0</v>
-      </c>
-      <c r="CN3" s="14">
-        <v>0</v>
-      </c>
-      <c r="CO3" s="14"/>
-      <c r="CP3" s="14"/>
-      <c r="CQ3" s="14"/>
-      <c r="CR3" s="14"/>
-      <c r="CS3" s="14">
-        <v>0</v>
-      </c>
-      <c r="CT3" s="14">
-        <v>0</v>
-      </c>
-      <c r="CU3" s="14">
-        <v>0</v>
-      </c>
-      <c r="CV3" s="14"/>
-      <c r="CW3" s="14"/>
-      <c r="CX3" s="14"/>
-      <c r="CY3" s="14">
-        <v>0</v>
-      </c>
-      <c r="CZ3" s="14"/>
-      <c r="DA3" s="14">
-        <v>0</v>
-      </c>
-      <c r="DB3" s="14">
-        <v>0</v>
-      </c>
-      <c r="DC3" s="14"/>
-      <c r="DD3" s="14"/>
-      <c r="DE3" s="14"/>
-      <c r="DF3" s="14">
-        <v>0</v>
-      </c>
-      <c r="DG3" s="14"/>
-      <c r="DH3" s="14">
-        <v>0</v>
-      </c>
-      <c r="DI3" s="14">
-        <v>0</v>
-      </c>
-      <c r="DJ3" s="14"/>
-      <c r="DK3" s="14"/>
-      <c r="DL3" s="14"/>
-      <c r="DM3" s="14"/>
-      <c r="DN3" s="14">
-        <v>0</v>
-      </c>
-      <c r="DO3" s="14">
-        <v>0</v>
-      </c>
-      <c r="DP3" s="1"/>
-      <c r="DQ3" s="1"/>
-      <c r="DR3" s="1"/>
-      <c r="DS3" s="1"/>
-      <c r="DT3" s="1"/>
-      <c r="DU3" s="1"/>
-      <c r="DV3" s="1"/>
-      <c r="DW3" s="1"/>
-      <c r="DX3" s="1"/>
-      <c r="DY3" s="1"/>
+      <c r="CG3" s="1"/>
+      <c r="CH3" s="1"/>
+      <c r="CI3" s="1"/>
+      <c r="CJ3" s="1"/>
+      <c r="CK3" s="1"/>
+      <c r="CL3" s="1"/>
+      <c r="CM3" s="1"/>
+      <c r="CN3" s="1"/>
+      <c r="CO3" s="1"/>
     </row>
-    <row r="4" spans="1:129" ht="50" customHeight="1">
+    <row r="4" spans="1:93" ht="50" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2">
         <f>F4-E4</f>
@@ -1592,7 +1403,7 @@
         <v>45436</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -1683,61 +1494,25 @@
       <c r="CD4" s="15"/>
       <c r="CE4" s="14"/>
       <c r="CF4" s="14"/>
-      <c r="CG4" s="14"/>
-      <c r="CH4" s="14"/>
-      <c r="CI4" s="14"/>
-      <c r="CJ4" s="14"/>
-      <c r="CK4" s="14"/>
-      <c r="CL4" s="14"/>
-      <c r="CM4" s="14"/>
-      <c r="CN4" s="14"/>
-      <c r="CO4" s="14"/>
-      <c r="CP4" s="14"/>
-      <c r="CQ4" s="14"/>
-      <c r="CR4" s="14"/>
-      <c r="CS4" s="14"/>
-      <c r="CT4" s="14"/>
-      <c r="CU4" s="14"/>
-      <c r="CV4" s="14"/>
-      <c r="CW4" s="14"/>
-      <c r="CX4" s="14"/>
-      <c r="CY4" s="14"/>
-      <c r="CZ4" s="14"/>
-      <c r="DA4" s="14"/>
-      <c r="DB4" s="14"/>
-      <c r="DC4" s="14"/>
-      <c r="DD4" s="14"/>
-      <c r="DE4" s="14"/>
-      <c r="DF4" s="14"/>
-      <c r="DG4" s="14"/>
-      <c r="DH4" s="14"/>
-      <c r="DI4" s="14"/>
-      <c r="DJ4" s="14"/>
-      <c r="DK4" s="14"/>
-      <c r="DL4" s="14"/>
-      <c r="DM4" s="14"/>
-      <c r="DN4" s="14"/>
-      <c r="DO4" s="14"/>
-      <c r="DP4" s="1"/>
-      <c r="DQ4" s="1"/>
-      <c r="DR4" s="1"/>
-      <c r="DS4" s="1"/>
-      <c r="DT4" s="1"/>
-      <c r="DU4" s="1"/>
-      <c r="DV4" s="1"/>
-      <c r="DW4" s="1"/>
-      <c r="DX4" s="1"/>
-      <c r="DY4" s="1"/>
+      <c r="CG4" s="1"/>
+      <c r="CH4" s="1"/>
+      <c r="CI4" s="1"/>
+      <c r="CJ4" s="1"/>
+      <c r="CK4" s="1"/>
+      <c r="CL4" s="1"/>
+      <c r="CM4" s="1"/>
+      <c r="CN4" s="1"/>
+      <c r="CO4" s="1"/>
     </row>
-    <row r="5" spans="1:129" ht="50" customHeight="1">
+    <row r="5" spans="1:93" ht="50" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2">
         <f>F5-E5</f>
@@ -1750,7 +1525,7 @@
         <v>45445</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -1847,61 +1622,25 @@
       <c r="CD5" s="15"/>
       <c r="CE5" s="14"/>
       <c r="CF5" s="14"/>
-      <c r="CG5" s="14"/>
-      <c r="CH5" s="14"/>
-      <c r="CI5" s="14"/>
-      <c r="CJ5" s="14"/>
-      <c r="CK5" s="14"/>
-      <c r="CL5" s="14"/>
-      <c r="CM5" s="14"/>
-      <c r="CN5" s="14"/>
-      <c r="CO5" s="14"/>
-      <c r="CP5" s="14"/>
-      <c r="CQ5" s="14"/>
-      <c r="CR5" s="14"/>
-      <c r="CS5" s="14"/>
-      <c r="CT5" s="14"/>
-      <c r="CU5" s="14"/>
-      <c r="CV5" s="14"/>
-      <c r="CW5" s="14"/>
-      <c r="CX5" s="14"/>
-      <c r="CY5" s="14"/>
-      <c r="CZ5" s="14"/>
-      <c r="DA5" s="14"/>
-      <c r="DB5" s="14"/>
-      <c r="DC5" s="14"/>
-      <c r="DD5" s="14"/>
-      <c r="DE5" s="14"/>
-      <c r="DF5" s="14"/>
-      <c r="DG5" s="14"/>
-      <c r="DH5" s="14"/>
-      <c r="DI5" s="14"/>
-      <c r="DJ5" s="14"/>
-      <c r="DK5" s="14"/>
-      <c r="DL5" s="14"/>
-      <c r="DM5" s="14"/>
-      <c r="DN5" s="14"/>
-      <c r="DO5" s="14"/>
-      <c r="DP5" s="1"/>
-      <c r="DQ5" s="1"/>
-      <c r="DR5" s="1"/>
-      <c r="DS5" s="1"/>
-      <c r="DT5" s="1"/>
-      <c r="DU5" s="1"/>
-      <c r="DV5" s="1"/>
-      <c r="DW5" s="1"/>
-      <c r="DX5" s="1"/>
-      <c r="DY5" s="1"/>
+      <c r="CG5" s="1"/>
+      <c r="CH5" s="1"/>
+      <c r="CI5" s="1"/>
+      <c r="CJ5" s="1"/>
+      <c r="CK5" s="1"/>
+      <c r="CL5" s="1"/>
+      <c r="CM5" s="1"/>
+      <c r="CN5" s="1"/>
+      <c r="CO5" s="1"/>
     </row>
-    <row r="6" spans="1:129" ht="50" customHeight="1">
+    <row r="6" spans="1:93" ht="50" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2">
         <f>F6-E6</f>
@@ -1914,7 +1653,7 @@
         <v>45452</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -2009,61 +1748,25 @@
       <c r="CD6" s="17"/>
       <c r="CE6" s="14"/>
       <c r="CF6" s="14"/>
-      <c r="CG6" s="14"/>
-      <c r="CH6" s="14"/>
-      <c r="CI6" s="14"/>
-      <c r="CJ6" s="14"/>
-      <c r="CK6" s="14"/>
-      <c r="CL6" s="14"/>
-      <c r="CM6" s="14"/>
-      <c r="CN6" s="14"/>
-      <c r="CO6" s="14"/>
-      <c r="CP6" s="14"/>
-      <c r="CQ6" s="14"/>
-      <c r="CR6" s="14"/>
-      <c r="CS6" s="14"/>
-      <c r="CT6" s="14"/>
-      <c r="CU6" s="14"/>
-      <c r="CV6" s="14"/>
-      <c r="CW6" s="14"/>
-      <c r="CX6" s="14"/>
-      <c r="CY6" s="14"/>
-      <c r="CZ6" s="14"/>
-      <c r="DA6" s="14"/>
-      <c r="DB6" s="14"/>
-      <c r="DC6" s="14"/>
-      <c r="DD6" s="14"/>
-      <c r="DE6" s="14"/>
-      <c r="DF6" s="14"/>
-      <c r="DG6" s="14"/>
-      <c r="DH6" s="14"/>
-      <c r="DI6" s="14"/>
-      <c r="DJ6" s="14"/>
-      <c r="DK6" s="14"/>
-      <c r="DL6" s="14"/>
-      <c r="DM6" s="14"/>
-      <c r="DN6" s="14"/>
-      <c r="DO6" s="14"/>
-      <c r="DP6" s="1"/>
-      <c r="DQ6" s="1"/>
-      <c r="DR6" s="1"/>
-      <c r="DS6" s="1"/>
-      <c r="DT6" s="1"/>
-      <c r="DU6" s="1"/>
-      <c r="DV6" s="1"/>
-      <c r="DW6" s="1"/>
-      <c r="DX6" s="1"/>
-      <c r="DY6" s="1"/>
+      <c r="CG6" s="1"/>
+      <c r="CH6" s="1"/>
+      <c r="CI6" s="1"/>
+      <c r="CJ6" s="1"/>
+      <c r="CK6" s="1"/>
+      <c r="CL6" s="1"/>
+      <c r="CM6" s="1"/>
+      <c r="CN6" s="1"/>
+      <c r="CO6" s="1"/>
     </row>
-    <row r="7" spans="1:129" ht="50" customHeight="1">
+    <row r="7" spans="1:93" ht="50" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D7" s="2">
         <f>F7-E7</f>
@@ -2076,7 +1779,7 @@
         <v>45488</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -2237,61 +1940,25 @@
       <c r="CD7" s="17"/>
       <c r="CE7" s="14"/>
       <c r="CF7" s="14"/>
-      <c r="CG7" s="14"/>
-      <c r="CH7" s="14"/>
-      <c r="CI7" s="14"/>
-      <c r="CJ7" s="14"/>
-      <c r="CK7" s="14"/>
-      <c r="CL7" s="14"/>
-      <c r="CM7" s="14"/>
-      <c r="CN7" s="14"/>
-      <c r="CO7" s="14"/>
-      <c r="CP7" s="14"/>
-      <c r="CQ7" s="14"/>
-      <c r="CR7" s="14"/>
-      <c r="CS7" s="14"/>
-      <c r="CT7" s="14"/>
-      <c r="CU7" s="14"/>
-      <c r="CV7" s="14"/>
-      <c r="CW7" s="14"/>
-      <c r="CX7" s="14"/>
-      <c r="CY7" s="14"/>
-      <c r="CZ7" s="14"/>
-      <c r="DA7" s="14"/>
-      <c r="DB7" s="14"/>
-      <c r="DC7" s="14"/>
-      <c r="DD7" s="14"/>
-      <c r="DE7" s="14"/>
-      <c r="DF7" s="14"/>
-      <c r="DG7" s="14"/>
-      <c r="DH7" s="14"/>
-      <c r="DI7" s="14"/>
-      <c r="DJ7" s="14"/>
-      <c r="DK7" s="14"/>
-      <c r="DL7" s="14"/>
-      <c r="DM7" s="14"/>
-      <c r="DN7" s="14"/>
-      <c r="DO7" s="14"/>
-      <c r="DP7" s="1"/>
-      <c r="DQ7" s="1"/>
-      <c r="DR7" s="1"/>
-      <c r="DS7" s="1"/>
-      <c r="DT7" s="1"/>
-      <c r="DU7" s="1"/>
-      <c r="DV7" s="1"/>
-      <c r="DW7" s="1"/>
-      <c r="DX7" s="1"/>
-      <c r="DY7" s="1"/>
+      <c r="CG7" s="1"/>
+      <c r="CH7" s="1"/>
+      <c r="CI7" s="1"/>
+      <c r="CJ7" s="1"/>
+      <c r="CK7" s="1"/>
+      <c r="CL7" s="1"/>
+      <c r="CM7" s="1"/>
+      <c r="CN7" s="1"/>
+      <c r="CO7" s="1"/>
     </row>
-    <row r="8" spans="1:129" ht="50" customHeight="1">
+    <row r="8" spans="1:93" ht="50" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2">
         <f>F8-E8</f>
@@ -2304,7 +1971,7 @@
         <v>45452</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H8" s="14">
         <v>0</v>
@@ -2469,81 +2136,16 @@
       <c r="CF8" s="14">
         <v>0</v>
       </c>
-      <c r="CG8" s="14">
-        <v>0</v>
-      </c>
-      <c r="CH8" s="14"/>
-      <c r="CI8" s="14"/>
-      <c r="CJ8" s="14"/>
-      <c r="CK8" s="14"/>
-      <c r="CL8" s="14">
-        <v>0</v>
-      </c>
-      <c r="CM8" s="14">
-        <v>0</v>
-      </c>
-      <c r="CN8" s="14">
-        <v>0</v>
-      </c>
-      <c r="CO8" s="14"/>
-      <c r="CP8" s="14"/>
-      <c r="CQ8" s="14"/>
-      <c r="CR8" s="14"/>
-      <c r="CS8" s="14">
-        <v>0</v>
-      </c>
-      <c r="CT8" s="14">
-        <v>0</v>
-      </c>
-      <c r="CU8" s="14">
-        <v>0</v>
-      </c>
-      <c r="CV8" s="14"/>
-      <c r="CW8" s="14"/>
-      <c r="CX8" s="14"/>
-      <c r="CY8" s="14">
-        <v>0</v>
-      </c>
-      <c r="CZ8" s="14"/>
-      <c r="DA8" s="14">
-        <v>0</v>
-      </c>
-      <c r="DB8" s="14">
-        <v>0</v>
-      </c>
-      <c r="DC8" s="14"/>
-      <c r="DD8" s="14"/>
-      <c r="DE8" s="14"/>
-      <c r="DF8" s="14">
-        <v>0</v>
-      </c>
-      <c r="DG8" s="14"/>
-      <c r="DH8" s="14">
-        <v>0</v>
-      </c>
-      <c r="DI8" s="14">
-        <v>0</v>
-      </c>
-      <c r="DJ8" s="14"/>
-      <c r="DK8" s="14"/>
-      <c r="DL8" s="14"/>
-      <c r="DM8" s="14"/>
-      <c r="DN8" s="14">
-        <v>0</v>
-      </c>
-      <c r="DO8" s="14">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:129" ht="50" customHeight="1">
+    <row r="9" spans="1:93" ht="50" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2">
         <f>F9-E9</f>
@@ -2556,7 +2158,7 @@
         <v>45480</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2701,51 +2303,16 @@
       <c r="CD9" s="14"/>
       <c r="CE9" s="17"/>
       <c r="CF9" s="17"/>
-      <c r="CG9" s="17"/>
-      <c r="CH9" s="17"/>
-      <c r="CI9" s="17"/>
-      <c r="CJ9" s="17"/>
-      <c r="CK9" s="17"/>
-      <c r="CL9" s="17"/>
-      <c r="CM9" s="17"/>
-      <c r="CN9" s="17"/>
-      <c r="CO9" s="17"/>
-      <c r="CP9" s="17"/>
-      <c r="CQ9" s="17"/>
-      <c r="CR9" s="17"/>
-      <c r="CS9" s="17"/>
-      <c r="CT9" s="17"/>
-      <c r="CU9" s="17"/>
-      <c r="CV9" s="17"/>
-      <c r="CW9" s="17"/>
-      <c r="CX9" s="17"/>
-      <c r="CY9" s="17"/>
-      <c r="CZ9" s="17"/>
-      <c r="DA9" s="17"/>
-      <c r="DB9" s="17"/>
-      <c r="DC9" s="17"/>
-      <c r="DD9" s="17"/>
-      <c r="DE9" s="17"/>
-      <c r="DF9" s="17"/>
-      <c r="DG9" s="17"/>
-      <c r="DH9" s="17"/>
-      <c r="DI9" s="17"/>
-      <c r="DJ9" s="17"/>
-      <c r="DK9" s="17"/>
-      <c r="DL9" s="17"/>
-      <c r="DM9" s="17"/>
-      <c r="DN9" s="17"/>
-      <c r="DO9" s="17"/>
     </row>
-    <row r="10" spans="1:129" ht="50" customHeight="1">
+    <row r="10" spans="1:93" ht="50" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2">
         <f>F10-E10</f>
@@ -2758,7 +2325,7 @@
         <v>45461</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H10" s="14">
         <v>0</v>
@@ -2927,82 +2494,16 @@
       <c r="CF10" s="14">
         <v>0</v>
       </c>
-      <c r="CG10" s="14">
-        <v>0</v>
-      </c>
-      <c r="CH10" s="14"/>
-      <c r="CI10" s="14"/>
-      <c r="CJ10" s="14"/>
-      <c r="CK10" s="14"/>
-      <c r="CL10" s="14">
-        <v>0</v>
-      </c>
-      <c r="CM10" s="14">
-        <v>0</v>
-      </c>
-      <c r="CN10" s="14">
-        <v>0</v>
-      </c>
-      <c r="CO10" s="14"/>
-      <c r="CP10" s="14"/>
-      <c r="CQ10" s="14"/>
-      <c r="CR10" s="14"/>
-      <c r="CS10" s="14">
-        <v>0</v>
-      </c>
-      <c r="CT10" s="14">
-        <v>0</v>
-      </c>
-      <c r="CU10" s="14">
-        <v>0</v>
-      </c>
-      <c r="CV10" s="14"/>
-      <c r="CW10" s="14"/>
-      <c r="CX10" s="14"/>
-      <c r="CY10" s="14">
-        <v>0</v>
-      </c>
-      <c r="CZ10" s="14"/>
-      <c r="DA10" s="14">
-        <v>0</v>
-      </c>
-      <c r="DB10" s="14">
-        <v>0</v>
-      </c>
-      <c r="DC10" s="14"/>
-      <c r="DD10" s="14"/>
-      <c r="DE10" s="14"/>
-      <c r="DF10" s="14">
-        <v>0</v>
-      </c>
-      <c r="DG10" s="14"/>
-      <c r="DH10" s="14">
-        <v>0</v>
-      </c>
-      <c r="DI10" s="14">
-        <v>0</v>
-      </c>
-      <c r="DJ10" s="14"/>
-      <c r="DK10" s="14"/>
-      <c r="DL10" s="14"/>
-      <c r="DM10" s="14"/>
-      <c r="DN10" s="14">
-        <v>0</v>
-      </c>
-      <c r="DO10" s="14">
-        <v>0</v>
-      </c>
-      <c r="DP10" s="1"/>
     </row>
-    <row r="11" spans="1:129" ht="50" customHeight="1">
+    <row r="11" spans="1:93" ht="50" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2">
         <f>F11-E11</f>
@@ -3015,7 +2516,7 @@
         <v>45488</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H11" s="14">
         <v>0</v>
@@ -3192,82 +2693,16 @@
       <c r="CF11" s="14">
         <v>0</v>
       </c>
-      <c r="CG11" s="14">
-        <v>0</v>
-      </c>
-      <c r="CH11" s="14"/>
-      <c r="CI11" s="14"/>
-      <c r="CJ11" s="14"/>
-      <c r="CK11" s="14"/>
-      <c r="CL11" s="14">
-        <v>0</v>
-      </c>
-      <c r="CM11" s="14">
-        <v>0</v>
-      </c>
-      <c r="CN11" s="14">
-        <v>0</v>
-      </c>
-      <c r="CO11" s="14"/>
-      <c r="CP11" s="14"/>
-      <c r="CQ11" s="14"/>
-      <c r="CR11" s="14"/>
-      <c r="CS11" s="14">
-        <v>0</v>
-      </c>
-      <c r="CT11" s="14">
-        <v>0</v>
-      </c>
-      <c r="CU11" s="14">
-        <v>0</v>
-      </c>
-      <c r="CV11" s="14"/>
-      <c r="CW11" s="14"/>
-      <c r="CX11" s="14"/>
-      <c r="CY11" s="14">
-        <v>0</v>
-      </c>
-      <c r="CZ11" s="14"/>
-      <c r="DA11" s="14">
-        <v>0</v>
-      </c>
-      <c r="DB11" s="14">
-        <v>0</v>
-      </c>
-      <c r="DC11" s="14"/>
-      <c r="DD11" s="14"/>
-      <c r="DE11" s="14"/>
-      <c r="DF11" s="14">
-        <v>0</v>
-      </c>
-      <c r="DG11" s="14"/>
-      <c r="DH11" s="14">
-        <v>0</v>
-      </c>
-      <c r="DI11" s="14">
-        <v>0</v>
-      </c>
-      <c r="DJ11" s="14"/>
-      <c r="DK11" s="14"/>
-      <c r="DL11" s="14"/>
-      <c r="DM11" s="14"/>
-      <c r="DN11" s="14">
-        <v>0</v>
-      </c>
-      <c r="DO11" s="14">
-        <v>0</v>
-      </c>
-      <c r="DP11" s="1"/>
     </row>
-    <row r="12" spans="1:129" ht="50" customHeight="1">
+    <row r="12" spans="1:93" ht="50" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2">
         <f>F12-E12</f>
@@ -3280,7 +2715,7 @@
         <v>45488</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H12" s="14">
         <v>0</v>
@@ -3451,81 +2886,16 @@
       <c r="CF12" s="14">
         <v>0</v>
       </c>
-      <c r="CG12" s="14">
-        <v>0</v>
-      </c>
-      <c r="CH12" s="14"/>
-      <c r="CI12" s="14"/>
-      <c r="CJ12" s="14"/>
-      <c r="CK12" s="14"/>
-      <c r="CL12" s="14">
-        <v>0</v>
-      </c>
-      <c r="CM12" s="14">
-        <v>0</v>
-      </c>
-      <c r="CN12" s="14">
-        <v>0</v>
-      </c>
-      <c r="CO12" s="14"/>
-      <c r="CP12" s="14"/>
-      <c r="CQ12" s="14"/>
-      <c r="CR12" s="14"/>
-      <c r="CS12" s="14">
-        <v>0</v>
-      </c>
-      <c r="CT12" s="14">
-        <v>0</v>
-      </c>
-      <c r="CU12" s="14">
-        <v>0</v>
-      </c>
-      <c r="CV12" s="14"/>
-      <c r="CW12" s="14"/>
-      <c r="CX12" s="14"/>
-      <c r="CY12" s="14">
-        <v>0</v>
-      </c>
-      <c r="CZ12" s="14"/>
-      <c r="DA12" s="14">
-        <v>0</v>
-      </c>
-      <c r="DB12" s="14">
-        <v>0</v>
-      </c>
-      <c r="DC12" s="14"/>
-      <c r="DD12" s="14"/>
-      <c r="DE12" s="14"/>
-      <c r="DF12" s="14">
-        <v>0</v>
-      </c>
-      <c r="DG12" s="14"/>
-      <c r="DH12" s="14">
-        <v>0</v>
-      </c>
-      <c r="DI12" s="14">
-        <v>0</v>
-      </c>
-      <c r="DJ12" s="14"/>
-      <c r="DK12" s="14"/>
-      <c r="DL12" s="14"/>
-      <c r="DM12" s="14"/>
-      <c r="DN12" s="14">
-        <v>0</v>
-      </c>
-      <c r="DO12" s="14">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:129" ht="50" customHeight="1">
+    <row r="13" spans="1:93" ht="50" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2">
         <f>F13-E13</f>
@@ -3538,7 +2908,7 @@
         <v>45494</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H13" s="14">
         <v>0</v>
@@ -3701,81 +3071,16 @@
       <c r="CF13" s="14">
         <v>0</v>
       </c>
-      <c r="CG13" s="14">
-        <v>0</v>
-      </c>
-      <c r="CH13" s="14"/>
-      <c r="CI13" s="14"/>
-      <c r="CJ13" s="14"/>
-      <c r="CK13" s="14"/>
-      <c r="CL13" s="14">
-        <v>0</v>
-      </c>
-      <c r="CM13" s="14">
-        <v>0</v>
-      </c>
-      <c r="CN13" s="14">
-        <v>0</v>
-      </c>
-      <c r="CO13" s="14"/>
-      <c r="CP13" s="14"/>
-      <c r="CQ13" s="14"/>
-      <c r="CR13" s="14"/>
-      <c r="CS13" s="14">
-        <v>0</v>
-      </c>
-      <c r="CT13" s="14">
-        <v>0</v>
-      </c>
-      <c r="CU13" s="14">
-        <v>0</v>
-      </c>
-      <c r="CV13" s="14"/>
-      <c r="CW13" s="14"/>
-      <c r="CX13" s="14"/>
-      <c r="CY13" s="14">
-        <v>0</v>
-      </c>
-      <c r="CZ13" s="14"/>
-      <c r="DA13" s="14">
-        <v>0</v>
-      </c>
-      <c r="DB13" s="14">
-        <v>0</v>
-      </c>
-      <c r="DC13" s="14"/>
-      <c r="DD13" s="14"/>
-      <c r="DE13" s="14"/>
-      <c r="DF13" s="14">
-        <v>0</v>
-      </c>
-      <c r="DG13" s="14"/>
-      <c r="DH13" s="14">
-        <v>0</v>
-      </c>
-      <c r="DI13" s="14">
-        <v>0</v>
-      </c>
-      <c r="DJ13" s="14"/>
-      <c r="DK13" s="14"/>
-      <c r="DL13" s="14"/>
-      <c r="DM13" s="14"/>
-      <c r="DN13" s="14">
-        <v>0</v>
-      </c>
-      <c r="DO13" s="14">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:129" ht="50" customHeight="1">
+    <row r="14" spans="1:93" ht="50" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2">
         <f>F14-E14</f>
@@ -3939,123 +3244,19 @@
       <c r="CF14" s="15">
         <v>0</v>
       </c>
-      <c r="CG14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CH14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CI14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CJ14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CK14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CL14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CM14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CN14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CO14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CP14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CQ14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CR14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CS14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CT14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CU14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CV14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CW14" s="15"/>
-      <c r="CX14" s="15"/>
-      <c r="CY14" s="15">
-        <v>0</v>
-      </c>
-      <c r="CZ14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DA14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DB14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DC14" s="15"/>
-      <c r="DD14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DE14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DF14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DG14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DH14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DI14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DJ14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DK14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DL14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DM14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DN14" s="15">
-        <v>0</v>
-      </c>
-      <c r="DO14" s="15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:129" ht="50" customHeight="1"/>
+    <row r="15" spans="1:93" ht="50" customHeight="1"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F14">
     <sortCondition ref="D2:D14"/>
   </sortState>
-  <mergeCells count="16">
-    <mergeCell ref="DI1:DO1"/>
+  <mergeCells count="11">
     <mergeCell ref="AQ1:AW1"/>
     <mergeCell ref="AX1:BD1"/>
     <mergeCell ref="BE1:BK1"/>
     <mergeCell ref="BL1:BR1"/>
     <mergeCell ref="BS1:BY1"/>
     <mergeCell ref="BZ1:CF1"/>
-    <mergeCell ref="CG1:CM1"/>
-    <mergeCell ref="CN1:CT1"/>
-    <mergeCell ref="CU1:DA1"/>
-    <mergeCell ref="DB1:DH1"/>
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="V1:AB1"/>
@@ -4064,27 +3265,27 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K2:AO2 H6:AO6 T7:AV7 H8:AO8 H9:BJ9 H10:AO12 BS2:CD2 BP6:CD6 CB7:CD7 BP8:CD12">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:DO14">
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:DO14">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
+  <conditionalFormatting sqref="H2:CF14">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:CF14">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:CF14">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="8" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>